<commit_message>
added old HOSVD code - just for testing
</commit_message>
<xml_diff>
--- a/rezultati.xlsx
+++ b/rezultati.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PMF\4.godina\2.semestar\MMP\seminar2\Tensor-Train-Decomposition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B812C80-C576-4280-9D3D-78150C4A55AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D699979-A59F-4284-9B65-6AE40606E21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{9520A465-0A6D-4DF7-BB11-834CC9FBA245}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9520A465-0A6D-4DF7-BB11-834CC9FBA245}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>TT3D</t>
   </si>
@@ -44,18 +44,6 @@
   </si>
   <si>
     <t>Least Squares</t>
-  </si>
-  <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
   </si>
   <si>
     <t>PROSJEK</t>
@@ -69,12 +57,15 @@
   <si>
     <t>MEDIAN</t>
   </si>
+  <si>
+    <t>HOSVD</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +102,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -142,110 +140,110 @@
     </border>
     <border>
       <left/>
-      <right style="dashDot">
+      <right style="dashDotDot">
         <color auto="1"/>
       </right>
       <top/>
-      <bottom style="dashDot">
+      <bottom style="dashDotDot">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="dashDot">
+      <left style="dashDotDot">
         <color auto="1"/>
       </left>
-      <right style="dashDot">
+      <right style="dashDotDot">
         <color auto="1"/>
       </right>
       <top/>
-      <bottom style="dashDot">
+      <bottom style="dashDotDot">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="dashDot">
+      <left style="dashDotDot">
         <color auto="1"/>
       </left>
       <right/>
       <top/>
-      <bottom style="dashDot">
+      <bottom style="dashDotDot">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="dashDot">
+      <right style="dashDotDot">
         <color auto="1"/>
       </right>
-      <top style="dashDot">
+      <top style="dashDotDot">
         <color auto="1"/>
       </top>
-      <bottom style="dashDot">
+      <bottom style="dashDotDot">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="dashDot">
+      <left style="dashDotDot">
         <color auto="1"/>
       </left>
-      <right style="dashDot">
+      <right style="dashDotDot">
         <color auto="1"/>
       </right>
-      <top style="dashDot">
+      <top style="dashDotDot">
         <color auto="1"/>
       </top>
-      <bottom style="dashDot">
+      <bottom style="dashDotDot">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="dashDot">
+      <left style="dashDotDot">
         <color auto="1"/>
       </left>
       <right/>
-      <top style="dashDot">
+      <top style="dashDotDot">
         <color auto="1"/>
       </top>
-      <bottom style="dashDot">
+      <bottom style="dashDotDot">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="dashDot">
+      <right style="dashDotDot">
         <color auto="1"/>
       </right>
-      <top style="dashDot">
+      <top style="dashDotDot">
         <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="dashDot">
+      <left style="dashDotDot">
         <color auto="1"/>
       </left>
-      <right style="dashDot">
+      <right style="dashDotDot">
         <color auto="1"/>
       </right>
-      <top style="dashDot">
+      <top style="dashDotDot">
         <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="dashDot">
+      <left style="dashDotDot">
         <color auto="1"/>
       </left>
       <right/>
-      <top style="dashDot">
+      <top style="dashDotDot">
         <color auto="1"/>
       </top>
       <bottom/>
@@ -256,7 +254,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -279,19 +277,25 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="10" fontId="2" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="4" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -609,20 +613,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8530D160-B7AA-431E-9ADD-D768C6A939F8}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -630,11 +634,14 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -644,11 +651,14 @@
       <c r="C2" s="5">
         <v>0.90272373540855999</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>0.904669260700389</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="6">
+        <v>0.90856000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -658,11 +668,14 @@
       <c r="C3" s="5">
         <v>0.92217898832684797</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>0.92996108949416401</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="6">
+        <v>0.92815999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -672,11 +685,14 @@
       <c r="C4" s="5">
         <v>0.91634241245136205</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>0.93385214007782102</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="6">
+        <v>0.92996100000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -686,11 +702,14 @@
       <c r="C5" s="5">
         <v>0.91439688715953304</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>0.92412451361867698</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="6">
+        <v>0.91827999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -700,11 +719,14 @@
       <c r="C6" s="5">
         <v>0.91828793774319095</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>0.90856031128404702</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="6">
+        <v>0.91439700000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -714,11 +736,14 @@
       <c r="C7" s="5">
         <v>0.90077821011673198</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>0.91439688715953304</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="6">
+        <v>0.90661500000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -728,11 +753,14 @@
       <c r="C8" s="5">
         <v>0.928015564202335</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>0.928015564202335</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="6">
+        <v>0.92996100000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -742,11 +770,14 @@
       <c r="C9" s="5">
         <v>0.91634241245136205</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>0.93385214007782102</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="6">
+        <v>0.92996100000000004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -756,11 +787,14 @@
       <c r="C10" s="5">
         <v>0.90661478599221801</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>0.91050583657587603</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="6">
+        <v>0.90446899999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -770,76 +804,95 @@
       <c r="C11" s="5">
         <v>0.91828793774319095</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>0.90856031128404702</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="6">
+        <v>0.91439700000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="9">
+        <v>3</v>
+      </c>
+      <c r="B12" s="8">
         <f>MIN(B2:B11)</f>
         <v>0.90077821011673198</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="8">
         <f>MIN(C2:C11)</f>
         <v>0.90077821011673198</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="9">
         <f>MIN(D2:D11)</f>
         <v>0.904669260700389</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="10">
+        <f>MIN(E2:E11)</f>
+        <v>0.90446899999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="9">
+        <v>4</v>
+      </c>
+      <c r="B13" s="8">
         <f>AVERAGE(B2:B11)</f>
         <v>0.91439688715953316</v>
       </c>
-      <c r="C13" s="9">
-        <f t="shared" ref="C13:D13" si="0">AVERAGE(C2:C11)</f>
+      <c r="C13" s="8">
+        <f t="shared" ref="C13:E13" si="0">AVERAGE(C2:C11)</f>
         <v>0.91439688715953316</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="9">
         <f t="shared" si="0"/>
         <v>0.9196498054474711</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="10">
+        <f t="shared" si="0"/>
+        <v>0.91847610000000013</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="9">
+        <v>5</v>
+      </c>
+      <c r="B14" s="8">
         <f>MAX(B2:B11)</f>
         <v>0.928015564202335</v>
       </c>
-      <c r="C14" s="9">
-        <f t="shared" ref="C14:D14" si="1">MAX(C2:C11)</f>
+      <c r="C14" s="8">
+        <f t="shared" ref="C14:E14" si="1">MAX(C2:C11)</f>
         <v>0.928015564202335</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="9">
         <f t="shared" si="1"/>
         <v>0.93385214007782102</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="10">
+      <c r="E14" s="10">
+        <f t="shared" si="1"/>
+        <v>0.92996100000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="12">
         <f>MEDIAN(B2:B11)</f>
         <v>0.91634241245136205</v>
       </c>
-      <c r="C15" s="10">
-        <f t="shared" ref="C15:D15" si="2">MEDIAN(C2:C11)</f>
+      <c r="C15" s="12">
+        <f t="shared" ref="C15:E15" si="2">MEDIAN(C2:C11)</f>
         <v>0.91634241245136205</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="13">
         <f t="shared" si="2"/>
         <v>0.91926070038910501</v>
+      </c>
+      <c r="E15" s="14">
+        <f t="shared" si="2"/>
+        <v>0.91633849999999994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>